<commit_message>
Checking in updated input
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDriver/TestRevenue/ActivityData_Apr22.xlsx
+++ b/src/test/resources/TestDriver/TestRevenue/ActivityData_Apr22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\TestRevenue (1)\TestRevenue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CD5EDC-2703-4924-A605-74473FF06479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E71CA0-B760-4DE5-9A99-A2CA0DDCC7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InstrumentAttribute" sheetId="1" r:id="rId1"/>
@@ -481,7 +481,9 @@
   </sheetPr>
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1447,13 +1449,13 @@
         <v>1</v>
       </c>
       <c r="H23" s="7">
-        <v>-4000</v>
+        <v>-1000</v>
       </c>
       <c r="I23" s="7">
         <v>1</v>
       </c>
       <c r="J23" s="7">
-        <v>-20000</v>
+        <v>-1000</v>
       </c>
       <c r="K23" s="5">
         <v>44576</v>
@@ -1491,13 +1493,13 @@
         <v>2</v>
       </c>
       <c r="H24" s="7">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="I24" s="7">
         <v>12</v>
       </c>
       <c r="J24" s="7">
-        <v>120000</v>
+        <v>6000</v>
       </c>
       <c r="K24" s="5">
         <v>44576</v>
@@ -1535,13 +1537,13 @@
         <v>3</v>
       </c>
       <c r="H25" s="7">
-        <v>6000</v>
+        <v>1500</v>
       </c>
       <c r="I25" s="7">
         <v>1</v>
       </c>
       <c r="J25" s="7">
-        <v>30000</v>
+        <v>1500</v>
       </c>
       <c r="K25" s="5">
         <v>44576</v>
@@ -1579,13 +1581,13 @@
         <v>5</v>
       </c>
       <c r="H26" s="7">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="I26" s="7">
         <v>24</v>
       </c>
       <c r="J26" s="7">
-        <v>24000</v>
+        <v>6000</v>
       </c>
       <c r="K26" s="5">
         <v>44576</v>

</xml_diff>